<commit_message>
Se mejora el formato fecha yyyy-mm-dd
</commit_message>
<xml_diff>
--- a/ETL/Estructura ETL.xlsx
+++ b/ETL/Estructura ETL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\richa\3D Objects\Project-Dengue\ETL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C46DEA18-FD9D-4B42-BBB9-9D8A04DED162}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{617A80DC-66B2-4F6F-8CC0-320C793AD13A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
@@ -66,9 +66,6 @@
     <t>Letalidad</t>
   </si>
   <si>
-    <t>Población_X_1000</t>
-  </si>
-  <si>
     <t>Argentina</t>
   </si>
   <si>
@@ -82,6 +79,9 @@
   </si>
   <si>
     <t>De 15 a 19 anos</t>
+  </si>
+  <si>
+    <t>Poblacion_X_1000</t>
   </si>
 </sst>
 </file>
@@ -490,7 +490,7 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75"/>
@@ -545,18 +545,18 @@
         <v>12</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="14.25">
       <c r="A2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="D2" s="4">
         <v>43466</v>
@@ -568,10 +568,10 @@
         <v>3</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="I2" s="1">
         <v>1</v>

</xml_diff>